<commit_message>
Updated with DNN with one hidden layer
</commit_message>
<xml_diff>
--- a/ClassifierEval.xlsx
+++ b/ClassifierEval.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kblongewicz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kblongewicz\Desktop\ParkingLots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E9C6B2DF-26B9-4C09-8228-A8FA784843B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC572893-1F13-46C5-8AFD-A6E16421C5D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20055" windowHeight="9435" xr2:uid="{E594CE4A-B0CD-4F52-8E16-C747FF49C3BF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20055" windowHeight="9435" activeTab="1" xr2:uid="{E594CE4A-B0CD-4F52-8E16-C747FF49C3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="89">
   <si>
     <t>Steps</t>
   </si>
@@ -313,7 +313,7 @@
     <numFmt numFmtId="166" formatCode="0.0000000"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +335,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -397,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -422,6 +428,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -11617,6 +11624,713 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DNNClassify.ipynb!$B$1248:$B$1324</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="77"/>
+                <c:pt idx="0">
+                  <c:v>92100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>276300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>368400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>460500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>552600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>644700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>736800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>828900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>921000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1013100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1105200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1197300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1289400</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1381500</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1473600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1565700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1657800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1749900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1842000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2026200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2118300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2210400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2302500</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2394600</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2486700</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2578800</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2670900</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2763000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2855100</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2947200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3039300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3131400</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3223500</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3315600</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3407700</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3499800</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3684000</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3776100</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3868200</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3960300</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4052400</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4144500</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4236600</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4328700</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4420800</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4512900</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4605000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4697100</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4789200</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4881300</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4973400</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5065500</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5157600</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5249700</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5341800</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5433900</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5526000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5618100</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5710200</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5802300</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5894400</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5986500</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6078600</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6262800</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6354900</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6447000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6539100</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6631200</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6723300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DNNClassify.ipynb!$C$1248:$C$1324</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="77"/>
+                <c:pt idx="0">
+                  <c:v>0.50361290000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61462665000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57871689999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61134224999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59229255000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59776660000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60740090000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63345739999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.65601050000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67221372999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68141012999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.69783229999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.71162689999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.72585940000000004</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.73965406</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75454350000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.76483469999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.76987079999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.77162253999999997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.77797240000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78629296999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.79045326000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.79527044000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.79789792999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.80030656</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.80380993999999995</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.80424786000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.80753229999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.80775123999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.80950295999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.81103570000000003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.81519600000000003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.81760454000000005</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.81891835000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.82132689999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.82417339999999994</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.82592509999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.82942850000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.83139914000000004</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.83161812999999996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.83271295000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.83358880000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.83424569999999998</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.83709215999999997</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.83971969999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.83971969999999996</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.84037660000000003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.84278520000000001</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.84409900000000004</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.84628859999999995</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.84694546000000004</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.84694546000000004</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.84672654000000003</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.84738340000000001</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.84869720000000004</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.85110574999999999</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.85110574999999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.85241955999999997</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.85285750000000005</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.85307639999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.85373330000000003</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.85460913000000005</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.85482809999999998</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.85548500000000005</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.85570394999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.85723669999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.85679877000000004</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.85833150000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.85789360000000003</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.85855049999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D28-449A-9D13-22B6EF2950EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="426772728"/>
+        <c:axId val="426774696"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="426772728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426774696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="426774696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426772728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -12245,7 +12959,589 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Run 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DNNClassify.ipynb!$B$43:$B$87</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>92200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>276600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>368800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>461000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>553200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>645400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>737600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>829800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>922000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1014200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1106400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1198600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1290800</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1383000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1475200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1567400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1659600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1751800</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1844000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1936200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2028400</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2120600</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2212800</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2305000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2397200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2489400</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2581600</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2673800</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2766000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2858200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2950400</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3042600</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3134800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3227000</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3319200</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3411400</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3503600</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3595800</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3688000</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3780200</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3872400</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3964600</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4056800</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4149000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DNNClassify.ipynb!$C$43:$C$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>0.56534030000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42096107999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38203957999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39726028000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44748858000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48858449999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52946293</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57295065999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.59404219999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.62600564999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.64535766999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.65644705000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66666669999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.67884319999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68732333000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.69167210000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69232439999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68993260000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.69580346000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68580127000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.67971300000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68427919999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.68384429999999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.69188950000000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.70450100000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.71972170000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.74472713000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.6449606</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.77886500000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79147639999999997</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.80104370000000003</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.80930639999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.8145249</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.81800390000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.82104809999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.82148295999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.82757119999999995</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.83061534000000004</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.83170253000000005</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.83365946999999996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.83496409999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.83496409999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.83670365999999996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.83779084999999998</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.83866059999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0883-45F5-A00B-DACC30AAC245}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="471253288"/>
+        <c:axId val="471253944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="471253288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="471253944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="471253944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="471253288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -12781,589 +14077,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Run 3</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>DNNClassify.ipynb!$B$43:$B$87</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>92200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>184400</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>276600</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>368800</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>461000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>553200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>645400</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>737600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>829800</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>922000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1014200</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1106400</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1198600</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1290800</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1383000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1475200</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1567400</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1659600</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1751800</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1844000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1936200</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2028400</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2120600</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2212800</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2305000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2397200</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2489400</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2581600</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2673800</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2766000</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2858200</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2950400</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3042600</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3134800</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3227000</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3319200</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3411400</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3503600</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3595800</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3688000</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3780200</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3872400</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3964600</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4056800</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>4149000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>DNNClassify.ipynb!$C$43:$C$87</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
-                <c:pt idx="0">
-                  <c:v>0.56534030000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.42096107999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.38203957999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39726028000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.44748858000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.48858449999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.52946293</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.57295065999999994</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.59404219999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.62600564999999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.64535766999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.65644705000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.66666669999999995</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.67884319999999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.68732333000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.69167210000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.69232439999999995</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.68993260000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.69580346000000004</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.68580127000000002</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.67971300000000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.68427919999999998</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.68384429999999996</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.69188950000000005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.70450100000000004</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.71972170000000002</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.74472713000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.6449606</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.77886500000000003</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.79147639999999997</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.80104370000000003</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.80930639999999998</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.8145249</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.81800390000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.82104809999999995</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.82148295999999998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.82757119999999995</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.83061534000000004</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.83170253000000005</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.83365946999999996</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.83496409999999999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.83496409999999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.83670365999999996</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.83779084999999998</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.83866059999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0883-45F5-A00B-DACC30AAC245}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="471253288"/>
-        <c:axId val="471253944"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="471253288"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="471253944"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="471253944"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="471253288"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -17884,6 +18598,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors31.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -29993,6 +30747,522 @@
 </file>
 
 <file path=xl/charts/style30.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style31.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -34590,6 +35860,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>577101</xdr:colOff>
+      <xdr:row>1299</xdr:row>
+      <xdr:rowOff>85166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>106454</xdr:colOff>
+      <xdr:row>1313</xdr:row>
+      <xdr:rowOff>161366</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="29" name="Chart 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C69CF82B-1CF8-4871-94E7-059047F33933}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -35061,8 +36367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12EB3099-EA53-402D-B317-53AC4D53931D}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36082,10 +37388,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1866225E-076A-4865-A822-37D5DFD185E4}">
-  <dimension ref="A1:D1247"/>
+  <dimension ref="A1:D1317"/>
   <sheetViews>
-    <sheetView topLeftCell="A1123" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1159" sqref="B1116:C1159"/>
+    <sheetView tabSelected="1" topLeftCell="A1300" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1317" sqref="D1317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46551,7 +47857,7 @@
         <v>0.68897724000000005</v>
       </c>
     </row>
-    <row r="1233" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1233" s="1">
         <v>2757000</v>
       </c>
@@ -46559,7 +47865,7 @@
         <v>0.68986080000000005</v>
       </c>
     </row>
-    <row r="1234" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1234" s="1">
         <v>2848900</v>
       </c>
@@ -46567,7 +47873,7 @@
         <v>0.69074440000000004</v>
       </c>
     </row>
-    <row r="1235" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1235" s="1">
         <v>2940800</v>
       </c>
@@ -46575,7 +47881,7 @@
         <v>0.69317430000000002</v>
       </c>
     </row>
-    <row r="1236" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1236" s="1">
         <v>3032700</v>
       </c>
@@ -46583,7 +47889,7 @@
         <v>0.69206979999999996</v>
       </c>
     </row>
-    <row r="1237" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1237" s="1">
         <v>3124600</v>
       </c>
@@ -46591,7 +47897,7 @@
         <v>0.6925116</v>
       </c>
     </row>
-    <row r="1238" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1238" s="1">
         <v>3216500</v>
       </c>
@@ -46599,7 +47905,7 @@
         <v>0.69184893000000003</v>
       </c>
     </row>
-    <row r="1239" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1239" s="1">
         <v>3308400</v>
       </c>
@@ -46607,7 +47913,7 @@
         <v>0.69206979999999996</v>
       </c>
     </row>
-    <row r="1240" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1240" s="1">
         <v>3400300</v>
       </c>
@@ -46615,7 +47921,7 @@
         <v>0.69405790000000001</v>
       </c>
     </row>
-    <row r="1241" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1241" s="1">
         <v>3492200</v>
       </c>
@@ -46623,7 +47929,7 @@
         <v>0.69494146000000001</v>
       </c>
     </row>
-    <row r="1242" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1242" s="1">
         <v>3584100</v>
       </c>
@@ -46631,7 +47937,7 @@
         <v>0.69604593999999997</v>
       </c>
     </row>
-    <row r="1243" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1243" s="1">
         <v>3676000</v>
       </c>
@@ -46639,7 +47945,7 @@
         <v>0.69604593999999997</v>
       </c>
     </row>
-    <row r="1244" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1244" s="1">
         <v>3767900</v>
       </c>
@@ -46647,7 +47953,7 @@
         <v>0.69715039999999995</v>
       </c>
     </row>
-    <row r="1245" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1245" s="1">
         <v>3859800</v>
       </c>
@@ -46655,7 +47961,7 @@
         <v>0.6975922</v>
       </c>
     </row>
-    <row r="1246" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1246" s="1">
         <v>3951700</v>
       </c>
@@ -46663,7 +47969,7 @@
         <v>0.69781309999999996</v>
       </c>
     </row>
-    <row r="1247" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1247" s="1">
         <v>4043600</v>
       </c>
@@ -46673,6 +47979,572 @@
       <c r="D1247">
         <f>MAX(C1204:C1247)</f>
         <v>0.69825493999999999</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1248" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1248" s="1">
+        <v>92100</v>
+      </c>
+      <c r="C1248">
+        <v>0.50361290000000003</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1249">
+        <v>34</v>
+      </c>
+      <c r="B1249" s="1">
+        <v>184200</v>
+      </c>
+      <c r="C1249">
+        <v>0.61462665000000005</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1250" s="1">
+        <v>276300</v>
+      </c>
+      <c r="C1250">
+        <v>0.57871689999999998</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1251" s="1">
+        <v>368400</v>
+      </c>
+      <c r="C1251">
+        <v>0.61134224999999998</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1252" s="1">
+        <v>460500</v>
+      </c>
+      <c r="C1252">
+        <v>0.59229255000000003</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1253" s="1">
+        <v>552600</v>
+      </c>
+      <c r="C1253">
+        <v>0.59776660000000004</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1254" s="1">
+        <v>644700</v>
+      </c>
+      <c r="C1254">
+        <v>0.60740090000000002</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1255" s="1">
+        <v>736800</v>
+      </c>
+      <c r="C1255">
+        <v>0.63345739999999995</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1256" s="1">
+        <v>828900</v>
+      </c>
+      <c r="C1256">
+        <v>0.65601050000000005</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1257" s="1">
+        <v>921000</v>
+      </c>
+      <c r="C1257">
+        <v>0.67221372999999995</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1258" s="1">
+        <v>1013100</v>
+      </c>
+      <c r="C1258">
+        <v>0.68141012999999995</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1259" s="1">
+        <v>1105200</v>
+      </c>
+      <c r="C1259">
+        <v>0.69783229999999996</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1260" s="1">
+        <v>1197300</v>
+      </c>
+      <c r="C1260">
+        <v>0.71162689999999995</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1261" s="1">
+        <v>1289400</v>
+      </c>
+      <c r="C1261">
+        <v>0.72585940000000004</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1262" s="1">
+        <v>1381500</v>
+      </c>
+      <c r="C1262">
+        <v>0.73965406</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1263" s="1">
+        <v>1473600</v>
+      </c>
+      <c r="C1263">
+        <v>0.75454350000000003</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1264" s="1">
+        <v>1565700</v>
+      </c>
+      <c r="C1264">
+        <v>0.76483469999999998</v>
+      </c>
+    </row>
+    <row r="1265" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1265" s="1">
+        <v>1657800</v>
+      </c>
+      <c r="C1265">
+        <v>0.76987079999999997</v>
+      </c>
+    </row>
+    <row r="1266" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1266" s="1">
+        <v>1749900</v>
+      </c>
+      <c r="C1266">
+        <v>0.77162253999999997</v>
+      </c>
+    </row>
+    <row r="1267" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1267" s="1">
+        <v>1842000</v>
+      </c>
+      <c r="C1267">
+        <v>0.77797240000000001</v>
+      </c>
+    </row>
+    <row r="1268" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1268" s="1">
+        <v>2026200</v>
+      </c>
+      <c r="C1268">
+        <v>0.78629296999999998</v>
+      </c>
+    </row>
+    <row r="1269" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1269" s="1">
+        <v>2118300</v>
+      </c>
+      <c r="C1269">
+        <v>0.79045326000000005</v>
+      </c>
+    </row>
+    <row r="1270" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1270" s="1">
+        <v>2210400</v>
+      </c>
+      <c r="C1270">
+        <v>0.79527044000000002</v>
+      </c>
+    </row>
+    <row r="1271" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1271" s="1">
+        <v>2302500</v>
+      </c>
+      <c r="C1271">
+        <v>0.79789792999999998</v>
+      </c>
+    </row>
+    <row r="1272" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1272" s="1">
+        <v>2394600</v>
+      </c>
+      <c r="C1272">
+        <v>0.80030656</v>
+      </c>
+    </row>
+    <row r="1273" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1273" s="1">
+        <v>2486700</v>
+      </c>
+      <c r="C1273">
+        <v>0.80380993999999995</v>
+      </c>
+    </row>
+    <row r="1274" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1274" s="1">
+        <v>2578800</v>
+      </c>
+      <c r="C1274">
+        <v>0.80424786000000004</v>
+      </c>
+    </row>
+    <row r="1275" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1275" s="1">
+        <v>2670900</v>
+      </c>
+      <c r="C1275">
+        <v>0.80753229999999998</v>
+      </c>
+    </row>
+    <row r="1276" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1276" s="1">
+        <v>2763000</v>
+      </c>
+      <c r="C1276">
+        <v>0.80775123999999998</v>
+      </c>
+    </row>
+    <row r="1277" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1277" s="1">
+        <v>2855100</v>
+      </c>
+      <c r="C1277">
+        <v>0.80950295999999999</v>
+      </c>
+    </row>
+    <row r="1278" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1278" s="1">
+        <v>2947200</v>
+      </c>
+      <c r="C1278">
+        <v>0.81103570000000003</v>
+      </c>
+    </row>
+    <row r="1279" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1279" s="1">
+        <v>3039300</v>
+      </c>
+      <c r="C1279">
+        <v>0.81519600000000003</v>
+      </c>
+    </row>
+    <row r="1280" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1280" s="1">
+        <v>3131400</v>
+      </c>
+      <c r="C1280">
+        <v>0.81760454000000005</v>
+      </c>
+    </row>
+    <row r="1281" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1281" s="1">
+        <v>3223500</v>
+      </c>
+      <c r="C1281">
+        <v>0.81891835000000002</v>
+      </c>
+    </row>
+    <row r="1282" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1282" s="1">
+        <v>3315600</v>
+      </c>
+      <c r="C1282">
+        <v>0.82132689999999997</v>
+      </c>
+    </row>
+    <row r="1283" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1283" s="1">
+        <v>3407700</v>
+      </c>
+      <c r="C1283">
+        <v>0.82417339999999994</v>
+      </c>
+    </row>
+    <row r="1284" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1284" s="1">
+        <v>3499800</v>
+      </c>
+      <c r="C1284">
+        <v>0.82592509999999997</v>
+      </c>
+    </row>
+    <row r="1285" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1285" s="1">
+        <v>3684000</v>
+      </c>
+      <c r="C1285">
+        <v>0.82942850000000001</v>
+      </c>
+    </row>
+    <row r="1286" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1286" s="1">
+        <v>3776100</v>
+      </c>
+      <c r="C1286">
+        <v>0.83139914000000004</v>
+      </c>
+    </row>
+    <row r="1287" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1287" s="1">
+        <v>3868200</v>
+      </c>
+      <c r="C1287">
+        <v>0.83161812999999996</v>
+      </c>
+    </row>
+    <row r="1288" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1288" s="1">
+        <v>3960300</v>
+      </c>
+      <c r="C1288">
+        <v>0.83271295000000001</v>
+      </c>
+    </row>
+    <row r="1289" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1289" s="1">
+        <v>4052400</v>
+      </c>
+      <c r="C1289" s="24">
+        <v>0.83358880000000002</v>
+      </c>
+    </row>
+    <row r="1290" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1290" s="1">
+        <v>4144500</v>
+      </c>
+      <c r="C1290">
+        <v>0.83424569999999998</v>
+      </c>
+    </row>
+    <row r="1291" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1291" s="1">
+        <v>4236600</v>
+      </c>
+      <c r="C1291">
+        <v>0.83709215999999997</v>
+      </c>
+    </row>
+    <row r="1292" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1292" s="1">
+        <v>4328700</v>
+      </c>
+      <c r="C1292">
+        <v>0.83971969999999996</v>
+      </c>
+    </row>
+    <row r="1293" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1293" s="1">
+        <v>4420800</v>
+      </c>
+      <c r="C1293">
+        <v>0.83971969999999996</v>
+      </c>
+    </row>
+    <row r="1294" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1294" s="1">
+        <v>4512900</v>
+      </c>
+      <c r="C1294">
+        <v>0.84037660000000003</v>
+      </c>
+    </row>
+    <row r="1295" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1295" s="1">
+        <v>4605000</v>
+      </c>
+      <c r="C1295">
+        <v>0.84278520000000001</v>
+      </c>
+    </row>
+    <row r="1296" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1296" s="1">
+        <v>4697100</v>
+      </c>
+      <c r="C1296">
+        <v>0.84409900000000004</v>
+      </c>
+    </row>
+    <row r="1297" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1297" s="1">
+        <v>4789200</v>
+      </c>
+      <c r="C1297">
+        <v>0.84628859999999995</v>
+      </c>
+    </row>
+    <row r="1298" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1298" s="1">
+        <v>4881300</v>
+      </c>
+      <c r="C1298">
+        <v>0.84694546000000004</v>
+      </c>
+    </row>
+    <row r="1299" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1299" s="1">
+        <v>4973400</v>
+      </c>
+      <c r="C1299">
+        <v>0.84694546000000004</v>
+      </c>
+    </row>
+    <row r="1300" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1300" s="1">
+        <v>5065500</v>
+      </c>
+      <c r="C1300">
+        <v>0.84672654000000003</v>
+      </c>
+    </row>
+    <row r="1301" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1301" s="1">
+        <v>5157600</v>
+      </c>
+      <c r="C1301">
+        <v>0.84738340000000001</v>
+      </c>
+    </row>
+    <row r="1302" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1302" s="1">
+        <v>5249700</v>
+      </c>
+      <c r="C1302">
+        <v>0.84869720000000004</v>
+      </c>
+    </row>
+    <row r="1303" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1303" s="1">
+        <v>5341800</v>
+      </c>
+      <c r="C1303">
+        <v>0.85110574999999999</v>
+      </c>
+    </row>
+    <row r="1304" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1304" s="1">
+        <v>5433900</v>
+      </c>
+      <c r="C1304">
+        <v>0.85110574999999999</v>
+      </c>
+    </row>
+    <row r="1305" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1305" s="1">
+        <v>5526000</v>
+      </c>
+      <c r="C1305">
+        <v>0.85241955999999997</v>
+      </c>
+    </row>
+    <row r="1306" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1306" s="1">
+        <v>5618100</v>
+      </c>
+      <c r="C1306">
+        <v>0.85285750000000005</v>
+      </c>
+    </row>
+    <row r="1307" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1307" s="1">
+        <v>5710200</v>
+      </c>
+      <c r="C1307">
+        <v>0.85307639999999996</v>
+      </c>
+    </row>
+    <row r="1308" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1308" s="1">
+        <v>5802300</v>
+      </c>
+      <c r="C1308">
+        <v>0.85373330000000003</v>
+      </c>
+    </row>
+    <row r="1309" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1309" s="1">
+        <v>5894400</v>
+      </c>
+      <c r="C1309">
+        <v>0.85460913000000005</v>
+      </c>
+    </row>
+    <row r="1310" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1310" s="1">
+        <v>5986500</v>
+      </c>
+      <c r="C1310">
+        <v>0.85482809999999998</v>
+      </c>
+    </row>
+    <row r="1311" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1311" s="1">
+        <v>6078600</v>
+      </c>
+      <c r="C1311">
+        <v>0.85548500000000005</v>
+      </c>
+    </row>
+    <row r="1312" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1312" s="1">
+        <v>6262800</v>
+      </c>
+      <c r="C1312">
+        <v>0.85570394999999999</v>
+      </c>
+    </row>
+    <row r="1313" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1313" s="1">
+        <v>6354900</v>
+      </c>
+      <c r="C1313">
+        <v>0.85723669999999996</v>
+      </c>
+    </row>
+    <row r="1314" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1314" s="1">
+        <v>6447000</v>
+      </c>
+      <c r="C1314">
+        <v>0.85679877000000004</v>
+      </c>
+    </row>
+    <row r="1315" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1315" s="1">
+        <v>6539100</v>
+      </c>
+      <c r="C1315">
+        <v>0.85833150000000002</v>
+      </c>
+    </row>
+    <row r="1316" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1316" s="1">
+        <v>6631200</v>
+      </c>
+      <c r="C1316">
+        <v>0.85789360000000003</v>
+      </c>
+    </row>
+    <row r="1317" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1317" s="1">
+        <v>6723300</v>
+      </c>
+      <c r="C1317">
+        <v>0.85855049999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>